<commit_message>
added more classes to the model(in progress).
</commit_message>
<xml_diff>
--- a/src/main/resources/soil_analysis_format.xlsx
+++ b/src/main/resources/soil_analysis_format.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\new\Desktop\year 3 sem 1\פרויקט\Final-Project-Maven\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Eviatar\IdeaProjects\Final-Project-Maven\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA043F0-0619-457C-92D0-46A6F6596357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11655"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="soil analysis" sheetId="3" r:id="rId1"/>
@@ -19,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>UOM</t>
   </si>
@@ -161,12 +157,27 @@
   </si>
   <si>
     <t>irrigation_block_id</t>
+  </si>
+  <si>
+    <t>Soil</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Silty_Clay</t>
+  </si>
+  <si>
+    <t>0-30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -320,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -350,6 +361,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -665,11 +679,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D41"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,153 +722,201 @@
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>42</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="B6" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="B7" s="11">
+        <v>43587</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="B8" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>29</v>
       </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
+      <c r="B14" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>12</v>
       </c>
@@ -911,12 +973,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1139,29 +1201,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E4B4E5-4FB0-4DD6-A95C-DC635ED5DF0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C030DB9-7096-45FC-9C50-E61F30C238BB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="766aba29-3875-45b2-af99-ed533f892980"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="aa781d43-3968-4c36-8c04-92512332ecb8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5144a9a3-a2b0-4147-97d3-94d65b917612"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1188,9 +1239,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C030DB9-7096-45FC-9C50-E61F30C238BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E4B4E5-4FB0-4DD6-A95C-DC635ED5DF0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="766aba29-3875-45b2-af99-ed533f892980"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="aa781d43-3968-4c36-8c04-92512332ecb8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5144a9a3-a2b0-4147-97d3-94d65b917612"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Model can now run without entering soil analysis/water analysis. Model can now run without errors when adding pre soil tables. Updated the database.
</commit_message>
<xml_diff>
--- a/src/main/resources/soil_analysis_format.xlsx
+++ b/src/main/resources/soil_analysis_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Eviatar\IdeaProjects\Final-Project-Maven\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA043F0-0619-457C-92D0-46A6F6596357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191733C8-DFCE-4706-B398-EC0CA1A7986C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>UOM</t>
   </si>
@@ -168,10 +168,73 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Silty_Clay</t>
-  </si>
-  <si>
     <t>0-30</t>
+  </si>
+  <si>
+    <t>Loam</t>
+  </si>
+  <si>
+    <t>2m KCl</t>
+  </si>
+  <si>
+    <t>Kjeldahl</t>
+  </si>
+  <si>
+    <t>Olsen</t>
+  </si>
+  <si>
+    <t>Ammonium Acetate</t>
+  </si>
+  <si>
+    <t>KCl 40</t>
+  </si>
+  <si>
+    <t>DTPA</t>
+  </si>
+  <si>
+    <t>Hot water</t>
+  </si>
+  <si>
+    <t>Ammonium Oxalate</t>
+  </si>
+  <si>
+    <t>Saturated paste</t>
+  </si>
+  <si>
+    <t>1M KCl</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>g/cm3</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>dS/m</t>
+  </si>
+  <si>
+    <t>Meq/100gr</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Meq/100g</t>
   </si>
 </sst>
 </file>
@@ -220,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -327,11 +390,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,6 +515,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -683,7 +864,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,6 +906,8 @@
       <c r="B2" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -733,14 +916,20 @@
       <c r="B3" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="2">
-        <v>1</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -749,6 +938,8 @@
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -757,14 +948,22 @@
       <c r="B6" s="2">
         <v>12</v>
       </c>
+      <c r="C6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="11">
-        <v>43587</v>
-      </c>
+        <v>42371</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -773,22 +972,30 @@
       <c r="B8" s="2">
         <v>11</v>
       </c>
+      <c r="C8" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -797,6 +1004,8 @@
       <c r="B11" s="2">
         <v>2</v>
       </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -805,6 +1014,10 @@
       <c r="B12" s="2">
         <v>0</v>
       </c>
+      <c r="C12" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -813,6 +1026,10 @@
       <c r="B13" s="2">
         <v>0</v>
       </c>
+      <c r="C13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -821,6 +1038,10 @@
       <c r="B14" s="2">
         <v>50</v>
       </c>
+      <c r="C14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -829,6 +1050,8 @@
       <c r="B15" s="2">
         <v>2</v>
       </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -837,133 +1060,341 @@
       <c r="B16" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>39</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed SOM calculation + summary calculation(for negative numbers). Updated the database(additional analysis records).
</commit_message>
<xml_diff>
--- a/src/main/resources/soil_analysis_format.xlsx
+++ b/src/main/resources/soil_analysis_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Eviatar\IdeaProjects\Final-Project-Maven\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191733C8-DFCE-4706-B398-EC0CA1A7986C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA931FB1-5899-4E7D-83D6-0DA4A241FAD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +924,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>59</v>
@@ -1012,7 +1012,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="2">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>61</v>
@@ -1024,7 +1024,7 @@
         <v>29</v>
       </c>
       <c r="B13" s="2">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>62</v>
@@ -1036,7 +1036,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>63</v>
@@ -1404,6 +1404,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1412,7 +1421,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E7F5E094DC5E2948848481730747906E" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e2ee9f7bc6b98ccdfe56e2ead30eeb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="766aba29-3875-45b2-af99-ed533f892980" xmlns:ns3="aa781d43-3968-4c36-8c04-92512332ecb8" xmlns:ns4="5144a9a3-a2b0-4147-97d3-94d65b917612" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4729878b84af48a8c52b489a8c554d66" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1631,16 +1640,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E4B4E5-4FB0-4DD6-A95C-DC635ED5DF0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="766aba29-3875-45b2-af99-ed533f892980"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="aa781d43-3968-4c36-8c04-92512332ecb8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5144a9a3-a2b0-4147-97d3-94d65b917612"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C030DB9-7096-45FC-9C50-E61F30C238BB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1648,7 +1667,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC88DF9A-5CBD-4A06-A933-7CDFE52F4587}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1667,23 +1686,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E4B4E5-4FB0-4DD6-A95C-DC635ED5DF0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="766aba29-3875-45b2-af99-ed533f892980"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="aa781d43-3968-4c36-8c04-92512332ecb8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5144a9a3-a2b0-4147-97d3-94d65b917612"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed Organic N extraction from excel table (id 20 instead of 15). Updated the database. Several minor changes in the model.
</commit_message>
<xml_diff>
--- a/src/main/resources/soil_analysis_format.xlsx
+++ b/src/main/resources/soil_analysis_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Eviatar\IdeaProjects\Final-Project-Maven\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA931FB1-5899-4E7D-83D6-0DA4A241FAD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BFF7F4-8565-4463-8D2E-67D44B31B5F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +924,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="2">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>59</v>
@@ -1082,7 +1082,7 @@
         <v>32</v>
       </c>
       <c r="B18" s="2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>66</v>
@@ -1096,7 +1096,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>66</v>
@@ -1110,7 +1110,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>66</v>
@@ -1124,7 +1124,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>66</v>
@@ -1138,7 +1138,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>66</v>
@@ -1152,7 +1152,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="2">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>66</v>
@@ -1166,7 +1166,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>65</v>
@@ -1180,7 +1180,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>65</v>
@@ -1194,7 +1194,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="2">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>66</v>
@@ -1208,7 +1208,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>66</v>
@@ -1222,7 +1222,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>66</v>
@@ -1236,7 +1236,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>66</v>
@@ -1278,7 +1278,7 @@
         <v>12</v>
       </c>
       <c r="B32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>66</v>
@@ -1404,15 +1404,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1421,7 +1412,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E7F5E094DC5E2948848481730747906E" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e2ee9f7bc6b98ccdfe56e2ead30eeb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="766aba29-3875-45b2-af99-ed533f892980" xmlns:ns3="aa781d43-3968-4c36-8c04-92512332ecb8" xmlns:ns4="5144a9a3-a2b0-4147-97d3-94d65b917612" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4729878b84af48a8c52b489a8c554d66" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1640,26 +1631,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E4B4E5-4FB0-4DD6-A95C-DC635ED5DF0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="766aba29-3875-45b2-af99-ed533f892980"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="aa781d43-3968-4c36-8c04-92512332ecb8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5144a9a3-a2b0-4147-97d3-94d65b917612"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C030DB9-7096-45FC-9C50-E61F30C238BB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1667,7 +1648,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC88DF9A-5CBD-4A06-A933-7CDFE52F4587}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1686,4 +1667,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E4B4E5-4FB0-4DD6-A95C-DC635ED5DF0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="766aba29-3875-45b2-af99-ed533f892980"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="aa781d43-3968-4c36-8c04-92512332ecb8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5144a9a3-a2b0-4147-97d3-94d65b917612"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>